<commit_message>
Solo falta ver el exportar
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>data</t>
   </si>
@@ -24,12 +24,12 @@
     <t>tipo</t>
   </si>
   <si>
+    <t>valor</t>
+  </si>
+  <si>
     <t>_id</t>
   </si>
   <si>
-    <t>valor</t>
-  </si>
-  <si>
     <t>permisos</t>
   </si>
   <si>
@@ -42,91 +42,55 @@
     <t>emailEmpresa</t>
   </si>
   <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>63bf788a7eab879ae1a110e9</t>
-  </si>
-  <si>
-    <t>Javier</t>
-  </si>
-  <si>
-    <t>63c4bcae7d405de464c87e4e</t>
-  </si>
-  <si>
-    <t>63bf796f7eab879ae1a111ce</t>
+    <t>name</t>
   </si>
   <si>
     <t>Nombre1</t>
   </si>
   <si>
+    <t>63c9d09535a6cb7859287813</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>Apellido1</t>
+  </si>
+  <si>
+    <t>63c9d09535a6cb7859287814</t>
+  </si>
+  <si>
+    <t>telefono</t>
+  </si>
+  <si>
+    <t>0997803371</t>
+  </si>
+  <si>
+    <t>63c9d09535a6cb7859287815</t>
+  </si>
+  <si>
     <t>Facturacion Electronica</t>
   </si>
   <si>
-    <t>Descripcion Facturacion Electronica</t>
-  </si>
-  <si>
-    <t>63bf6e877eab879ae1a1106c</t>
-  </si>
-  <si>
-    <t>18/1/2023</t>
-  </si>
-  <si>
-    <t>boris@Pichincha.com</t>
-  </si>
-  <si>
-    <t>63c093f2330bb509fffaed82</t>
-  </si>
-  <si>
-    <t>63c093a2330bb509fffaed24</t>
-  </si>
-  <si>
-    <t>Milann</t>
-  </si>
-  <si>
-    <t>63c4bcd77d405de464c87ecc</t>
+    <t>Descripción del uso que se dará</t>
+  </si>
+  <si>
+    <t>63c9cfc435a6cb78592877b3</t>
   </si>
   <si>
     <t>Marketing</t>
   </si>
   <si>
-    <t>Descripcion MArketing</t>
-  </si>
-  <si>
-    <t>63bf79567eab879ae1a1118a</t>
-  </si>
-  <si>
-    <t>20/1/2023</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>63c4c0147d405de464c8807d</t>
-  </si>
-  <si>
-    <t>direccion</t>
-  </si>
-  <si>
-    <t>63c4c1a17d405de464c88197</t>
-  </si>
-  <si>
-    <t>Tratamiento empresa2</t>
-  </si>
-  <si>
-    <t>27/1/2023</t>
-  </si>
-  <si>
-    <t>empresa2@hotmail.com</t>
-  </si>
-  <si>
-    <t>Direccion m</t>
-  </si>
-  <si>
-    <t>63c4c1a17d405de464c88198</t>
-  </si>
-  <si>
-    <t>Tratamiento Prueba</t>
+    <t>Descripcion de marketing</t>
+  </si>
+  <si>
+    <t>63c9cfc435a6cb78592877b4</t>
+  </si>
+  <si>
+    <t>31/1/2023</t>
+  </si>
+  <si>
+    <t>empresa1@hotmail.com</t>
   </si>
   <si>
     <t>Evaluation Only. Created with Aspose.Cells for Node.js via Java.Copyright 2003 - 2023 Aspose Pty Ltd.</t>
@@ -587,21 +551,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79ffd2a6-9631-48ea-8eb6-98597342747a}">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{d47d8235-be3d-4f38-9f3f-c039063c7af0}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.714285714285714" customWidth="1"/>
-    <col min="2" max="2" width="25.285714285714285" customWidth="1"/>
-    <col min="3" max="3" width="11.142857142857142" customWidth="1"/>
+    <col min="1" max="1" width="9.142857142857142" customWidth="1"/>
+    <col min="2" max="2" width="11.285714285714286" customWidth="1"/>
+    <col min="3" max="3" width="25.285714285714285" customWidth="1"/>
     <col min="4" max="4" width="20.857142857142858" customWidth="1"/>
     <col min="5" max="5" width="6.142857142857143" customWidth="1"/>
-    <col min="6" max="6" width="31.142857142857142" customWidth="1"/>
-    <col min="7" max="7" width="8.714285714285714" customWidth="1"/>
-    <col min="8" max="8" width="25.285714285714285" customWidth="1"/>
+    <col min="6" max="6" width="27.857142857142858" customWidth="1"/>
+    <col min="7" max="7" width="7.714285714285714" customWidth="1"/>
+    <col min="8" max="8" width="24.714285714285715" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
     <col min="10" max="10" width="21.428571428571427" customWidth="1"/>
   </cols>
@@ -640,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -649,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -665,167 +629,65 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12.75">
+    <row r="4" spans="1:8" ht="12.75">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="12.75">
+    <row r="5" spans="1:7" ht="12.75">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
         <v>14</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="12.75">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="12.75">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="12.75">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +702,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14a41689-956a-40c8-8712-1fb4fe4f4f54}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{b196533c-d9d4-4a3b-8d6a-4634b0471dc8}">
   <dimension ref="A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
@@ -849,7 +711,7 @@
   <sheetData>
     <row r="5" spans="1:1" ht="23.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>